<commit_message>
poes lls cpr phar
</commit_message>
<xml_diff>
--- a/QA/testcases/CPR/Pharmacy/Phar_Patient_App_Create_PCase_Positive_Alien_POE1.xlsx
+++ b/QA/testcases/CPR/Pharmacy/Phar_Patient_App_Create_PCase_Positive_Alien_POE1.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419">
   <si>
     <t>Step No</t>
   </si>
@@ -892,57 +892,6 @@
     <t>Create Expenditure clicked</t>
   </si>
   <si>
-    <t>CLAIM_SEARCH_PROVIDER</t>
-  </si>
-  <si>
-    <t>1.Existing provider search</t>
-  </si>
-  <si>
-    <t>NAME_TAB_ADD_PROVIDER</t>
-  </si>
-  <si>
-    <t>SEARCH_PROV_STATE</t>
-  </si>
-  <si>
-    <t>Alabama</t>
-  </si>
-  <si>
-    <t>Select State from the search popup</t>
-  </si>
-  <si>
-    <t>SEARCH_PROV_LASTNAME</t>
-  </si>
-  <si>
-    <t>Heller</t>
-  </si>
-  <si>
-    <t>SEARCH_PROV_SEARCH</t>
-  </si>
-  <si>
-    <t>Click Search button</t>
-  </si>
-  <si>
-    <t>Search clicked</t>
-  </si>
-  <si>
-    <t>SEARCH_PROV_SEARCH_FIRST</t>
-  </si>
-  <si>
-    <t>Select first provider</t>
-  </si>
-  <si>
-    <t>Provier selected</t>
-  </si>
-  <si>
-    <t>SEARCH_PROV_ADD_PROVIDER</t>
-  </si>
-  <si>
-    <t>Click Add Provider</t>
-  </si>
-  <si>
-    <t>Provider added</t>
-  </si>
-  <si>
     <t>EXPE_DATE_OF_SERVICE_FROM</t>
   </si>
   <si>
@@ -967,6 +916,9 @@
     <t>EXPE_ELECTRONIC_SIGN</t>
   </si>
   <si>
+    <t>1. Payable to Provider submitted</t>
+  </si>
+  <si>
     <t>Click ok to Pcase alert</t>
   </si>
   <si>
@@ -1040,15 +992,6 @@
   </si>
   <si>
     <t>CLAIM_PAYABLE_STATE</t>
-  </si>
-  <si>
-    <t>PATIENT_LOGOUT</t>
-  </si>
-  <si>
-    <t>Click on logout</t>
-  </si>
-  <si>
-    <t>Logout successfully</t>
   </si>
   <si>
     <t>Actions</t>
@@ -1347,10 +1290,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -1377,8 +1320,86 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1399,32 +1420,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1439,83 +1451,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1542,13 +1485,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1560,7 +1545,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1572,61 +1605,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1644,73 +1641,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1722,12 +1659,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1773,24 +1716,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color theme="4" tint="0.399975585192419"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4" tint="0.399975585192419"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4" tint="0.399975585192419"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1806,41 +1751,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1869,6 +1779,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1883,16 +1802,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1904,134 +1834,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2040,7 +1970,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2393,10 +2322,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:H251"/>
+  <dimension ref="A1:H214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A235" workbookViewId="0">
-      <selection activeCell="A250" sqref="$A250:$XFD250"/>
+    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
+      <selection activeCell="F188" sqref="F188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85714285714286" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -5430,7 +5359,7 @@
       <c r="G142" s="6"/>
       <c r="H142" s="6"/>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" s="4" customFormat="1" spans="1:8">
       <c r="A143" s="7">
         <v>142</v>
       </c>
@@ -5438,32 +5367,36 @@
         <v>14</v>
       </c>
       <c r="C143" s="7" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D143" s="7" t="s">
         <v>288</v>
       </c>
       <c r="E143" s="7"/>
-      <c r="F143" s="7" t="s">
-        <v>289</v>
-      </c>
+      <c r="F143" s="7"/>
       <c r="G143" s="7"/>
       <c r="H143" s="7"/>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" s="4" customFormat="1" spans="1:8">
       <c r="A144" s="6">
         <v>143</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C144" s="6"/>
-      <c r="D144" s="6"/>
-      <c r="E144" s="6">
-        <v>3</v>
-      </c>
-      <c r="F144" s="6"/>
-      <c r="G144" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="C144" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D144" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="E144" s="6"/>
+      <c r="F144" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G144" s="6" t="s">
+        <v>176</v>
+      </c>
       <c r="H144" s="6"/>
     </row>
     <row r="145" s="4" customFormat="1" spans="1:8">
@@ -5489,130 +5422,126 @@
         <v>145</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C146" s="6"/>
-      <c r="D146" s="6"/>
-      <c r="E146" s="6">
-        <v>1</v>
-      </c>
-      <c r="F146" s="6"/>
-      <c r="G146" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="C146" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D146" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E146" s="6"/>
+      <c r="F146" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G146" s="6" t="s">
+        <v>176</v>
+      </c>
       <c r="H146" s="6"/>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" s="4" customFormat="1" spans="1:8">
       <c r="A147" s="7">
         <v>146</v>
       </c>
       <c r="B147" s="7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C147" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D147" s="7" t="s">
-        <v>291</v>
-      </c>
-      <c r="E147" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="F147" s="7" t="s">
-        <v>293</v>
-      </c>
-      <c r="G147" s="7" t="s">
-        <v>105</v>
-      </c>
+      <c r="E147" s="7">
+        <v>200</v>
+      </c>
+      <c r="F147" s="7"/>
+      <c r="G147" s="7"/>
       <c r="H147" s="7"/>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" s="4" customFormat="1" spans="1:8">
       <c r="A148" s="6">
         <v>147</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="C148" s="6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D148" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="E148" s="6" t="s">
-        <v>295</v>
-      </c>
+        <v>293</v>
+      </c>
+      <c r="E148" s="6"/>
       <c r="F148" s="6" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="G148" s="6" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="H148" s="6"/>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" s="4" customFormat="1" spans="1:8">
       <c r="A149" s="7">
         <v>148</v>
       </c>
       <c r="B149" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C149" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D149" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="E149" s="7"/>
-      <c r="F149" s="7" t="s">
-        <v>297</v>
-      </c>
-      <c r="G149" s="7" t="s">
-        <v>298</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C149" s="7"/>
+      <c r="D149" s="7"/>
+      <c r="E149" s="7">
+        <v>3</v>
+      </c>
+      <c r="F149" s="7"/>
+      <c r="G149" s="7"/>
       <c r="H149" s="7"/>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" s="4" customFormat="1" spans="1:8">
       <c r="A150" s="6">
         <v>149</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C150" s="6"/>
-      <c r="D150" s="6"/>
-      <c r="E150" s="6">
-        <v>4</v>
-      </c>
-      <c r="F150" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G150" s="6" t="s">
-        <v>13</v>
-      </c>
+        <v>67</v>
+      </c>
+      <c r="C150" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D150" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="E150" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="F150" s="6"/>
+      <c r="G150" s="6"/>
       <c r="H150" s="6"/>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" s="4" customFormat="1" spans="1:8">
       <c r="A151" s="7">
         <v>150</v>
       </c>
       <c r="B151" s="7" t="s">
-        <v>14</v>
+        <v>271</v>
       </c>
       <c r="C151" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D151" s="7" t="s">
-        <v>299</v>
-      </c>
-      <c r="E151" s="7"/>
+        <v>272</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>273</v>
+      </c>
       <c r="F151" s="7" t="s">
-        <v>300</v>
+        <v>274</v>
       </c>
       <c r="G151" s="7" t="s">
-        <v>301</v>
+        <v>275</v>
       </c>
       <c r="H151" s="7"/>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" s="4" customFormat="1" spans="1:8">
       <c r="A152" s="6">
         <v>151</v>
       </c>
@@ -5623,18 +5552,18 @@
         <v>35</v>
       </c>
       <c r="D152" s="6" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="E152" s="6"/>
       <c r="F152" s="6" t="s">
-        <v>303</v>
+        <v>92</v>
       </c>
       <c r="G152" s="6" t="s">
-        <v>304</v>
+        <v>93</v>
       </c>
       <c r="H152" s="6"/>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" s="4" customFormat="1" spans="1:8">
       <c r="A153" s="7">
         <v>152</v>
       </c>
@@ -5644,7 +5573,7 @@
       <c r="C153" s="7"/>
       <c r="D153" s="7"/>
       <c r="E153" s="7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F153" s="7"/>
       <c r="G153" s="7"/>
@@ -5661,7 +5590,7 @@
         <v>35</v>
       </c>
       <c r="D154" s="6" t="s">
-        <v>305</v>
+        <v>294</v>
       </c>
       <c r="E154" s="6"/>
       <c r="F154" s="6"/>
@@ -5673,21 +5602,19 @@
         <v>154</v>
       </c>
       <c r="B155" s="7" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C155" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D155" s="7" t="s">
-        <v>306</v>
-      </c>
-      <c r="E155" s="7"/>
-      <c r="F155" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G155" s="7" t="s">
-        <v>176</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="F155" s="7"/>
+      <c r="G155" s="7"/>
       <c r="H155" s="7"/>
     </row>
     <row r="156" s="4" customFormat="1" spans="1:8">
@@ -5701,10 +5628,12 @@
         <v>35</v>
       </c>
       <c r="D156" s="6" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="E156" s="6"/>
-      <c r="F156" s="6"/>
+      <c r="F156" s="6" t="s">
+        <v>296</v>
+      </c>
       <c r="G156" s="6"/>
       <c r="H156" s="6"/>
     </row>
@@ -5713,21 +5642,15 @@
         <v>156</v>
       </c>
       <c r="B157" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C157" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D157" s="7" t="s">
-        <v>308</v>
-      </c>
-      <c r="E157" s="7"/>
-      <c r="F157" s="7" t="s">
-        <v>175</v>
-      </c>
-      <c r="G157" s="7" t="s">
-        <v>176</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C157" s="7"/>
+      <c r="D157" s="7"/>
+      <c r="E157" s="7">
+        <v>10</v>
+      </c>
+      <c r="F157" s="7"/>
+      <c r="G157" s="7"/>
       <c r="H157" s="7"/>
     </row>
     <row r="158" s="4" customFormat="1" spans="1:8">
@@ -5735,19 +5658,17 @@
         <v>157</v>
       </c>
       <c r="B158" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C158" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D158" s="6" t="s">
-        <v>309</v>
-      </c>
-      <c r="E158" s="6">
-        <v>200</v>
-      </c>
-      <c r="F158" s="6"/>
-      <c r="G158" s="6"/>
+        <v>278</v>
+      </c>
+      <c r="C158" s="6"/>
+      <c r="D158" s="6"/>
+      <c r="E158" s="6"/>
+      <c r="F158" s="6" t="s">
+        <v>297</v>
+      </c>
+      <c r="G158" s="6" t="s">
+        <v>298</v>
+      </c>
       <c r="H158" s="6"/>
     </row>
     <row r="159" s="4" customFormat="1" spans="1:8">
@@ -5755,21 +5676,15 @@
         <v>158</v>
       </c>
       <c r="B159" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C159" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D159" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="E159" s="7"/>
-      <c r="F159" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G159" s="7" t="s">
-        <v>93</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C159" s="7"/>
+      <c r="D159" s="7"/>
+      <c r="E159" s="7">
+        <v>10</v>
+      </c>
+      <c r="F159" s="7"/>
+      <c r="G159" s="7"/>
       <c r="H159" s="7"/>
     </row>
     <row r="160" s="4" customFormat="1" spans="1:8">
@@ -5777,15 +5692,21 @@
         <v>159</v>
       </c>
       <c r="B160" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C160" s="6"/>
-      <c r="D160" s="6"/>
-      <c r="E160" s="6">
-        <v>3</v>
-      </c>
-      <c r="F160" s="6"/>
-      <c r="G160" s="6"/>
+        <v>233</v>
+      </c>
+      <c r="C160" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D160" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="E160" s="6"/>
+      <c r="F160" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="G160" s="6" t="s">
+        <v>301</v>
+      </c>
       <c r="H160" s="6"/>
     </row>
     <row r="161" s="4" customFormat="1" spans="1:8">
@@ -5793,19 +5714,21 @@
         <v>160</v>
       </c>
       <c r="B161" s="7" t="s">
-        <v>67</v>
+        <v>302</v>
       </c>
       <c r="C161" s="7" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D161" s="7" t="s">
-        <v>263</v>
-      </c>
-      <c r="E161" s="7" t="s">
-        <v>264</v>
-      </c>
-      <c r="F161" s="7"/>
-      <c r="G161" s="7"/>
+        <v>303</v>
+      </c>
+      <c r="E161" s="7"/>
+      <c r="F161" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="G161" s="7" t="s">
+        <v>305</v>
+      </c>
       <c r="H161" s="7"/>
     </row>
     <row r="162" s="4" customFormat="1" spans="1:8">
@@ -5813,22 +5736,20 @@
         <v>161</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>271</v>
+        <v>14</v>
       </c>
       <c r="C162" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D162" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="E162" s="6" t="s">
-        <v>273</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="E162" s="6"/>
       <c r="F162" s="6" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="G162" s="6" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="H162" s="6"/>
     </row>
@@ -5837,21 +5758,15 @@
         <v>162</v>
       </c>
       <c r="B163" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C163" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D163" s="7" t="s">
-        <v>310</v>
-      </c>
-      <c r="E163" s="7"/>
-      <c r="F163" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="G163" s="7" t="s">
-        <v>93</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C163" s="7"/>
+      <c r="D163" s="7"/>
+      <c r="E163" s="7">
+        <v>5</v>
+      </c>
+      <c r="F163" s="7"/>
+      <c r="G163" s="7"/>
       <c r="H163" s="7"/>
     </row>
     <row r="164" s="4" customFormat="1" spans="1:8">
@@ -5859,15 +5774,23 @@
         <v>163</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C164" s="6"/>
-      <c r="D164" s="6"/>
-      <c r="E164" s="6">
-        <v>2</v>
-      </c>
-      <c r="F164" s="6"/>
-      <c r="G164" s="6"/>
+        <v>44</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D164" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="E164" s="6" t="s">
+        <v>307</v>
+      </c>
+      <c r="F164" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="G164" s="6" t="s">
+        <v>309</v>
+      </c>
       <c r="H164" s="6"/>
     </row>
     <row r="165" s="4" customFormat="1" spans="1:8">
@@ -5878,10 +5801,10 @@
         <v>14</v>
       </c>
       <c r="C165" s="7" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D165" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E165" s="7"/>
       <c r="F165" s="7"/>
@@ -5893,16 +5816,12 @@
         <v>165</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C166" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D166" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="E166" s="6" t="s">
-        <v>99</v>
+        <v>11</v>
+      </c>
+      <c r="C166" s="6"/>
+      <c r="D166" s="6"/>
+      <c r="E166" s="6">
+        <v>1</v>
       </c>
       <c r="F166" s="6"/>
       <c r="G166" s="6"/>
@@ -5913,15 +5832,17 @@
         <v>166</v>
       </c>
       <c r="B167" s="7" t="s">
-        <v>14</v>
+        <v>311</v>
       </c>
       <c r="C167" s="7" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D167" s="7" t="s">
-        <v>311</v>
-      </c>
-      <c r="E167" s="7"/>
+        <v>312</v>
+      </c>
+      <c r="E167" s="7">
+        <v>10002</v>
+      </c>
       <c r="F167" s="7"/>
       <c r="G167" s="7"/>
       <c r="H167" s="7"/>
@@ -5931,13 +5852,15 @@
         <v>167</v>
       </c>
       <c r="B168" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C168" s="6"/>
-      <c r="D168" s="6"/>
-      <c r="E168" s="6">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C168" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D168" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="E168" s="6"/>
       <c r="F168" s="6"/>
       <c r="G168" s="6"/>
       <c r="H168" s="6"/>
@@ -5947,17 +5870,15 @@
         <v>168</v>
       </c>
       <c r="B169" s="7" t="s">
-        <v>278</v>
+        <v>11</v>
       </c>
       <c r="C169" s="7"/>
       <c r="D169" s="7"/>
-      <c r="E169" s="7"/>
-      <c r="F169" s="7" t="s">
-        <v>313</v>
-      </c>
-      <c r="G169" s="7" t="s">
-        <v>314</v>
-      </c>
+      <c r="E169" s="7">
+        <v>1</v>
+      </c>
+      <c r="F169" s="7"/>
+      <c r="G169" s="7"/>
       <c r="H169" s="7"/>
     </row>
     <row r="170" s="4" customFormat="1" spans="1:8">
@@ -5965,13 +5886,15 @@
         <v>169</v>
       </c>
       <c r="B170" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C170" s="6"/>
-      <c r="D170" s="6"/>
-      <c r="E170" s="6">
-        <v>10</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="C170" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D170" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="E170" s="6"/>
       <c r="F170" s="6"/>
       <c r="G170" s="6"/>
       <c r="H170" s="6"/>
@@ -5981,21 +5904,17 @@
         <v>170</v>
       </c>
       <c r="B171" s="7" t="s">
-        <v>233</v>
+        <v>14</v>
       </c>
       <c r="C171" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D171" s="7" t="s">
-        <v>315</v>
+        <v>288</v>
       </c>
       <c r="E171" s="7"/>
-      <c r="F171" s="7" t="s">
-        <v>316</v>
-      </c>
-      <c r="G171" s="7" t="s">
-        <v>317</v>
-      </c>
+      <c r="F171" s="7"/>
+      <c r="G171" s="7"/>
       <c r="H171" s="7"/>
     </row>
     <row r="172" s="4" customFormat="1" spans="1:8">
@@ -6003,20 +5922,20 @@
         <v>171</v>
       </c>
       <c r="B172" s="6" t="s">
-        <v>318</v>
+        <v>14</v>
       </c>
       <c r="C172" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D172" s="6" t="s">
-        <v>319</v>
+        <v>289</v>
       </c>
       <c r="E172" s="6"/>
       <c r="F172" s="6" t="s">
-        <v>320</v>
+        <v>175</v>
       </c>
       <c r="G172" s="6" t="s">
-        <v>321</v>
+        <v>176</v>
       </c>
       <c r="H172" s="6"/>
     </row>
@@ -6031,15 +5950,11 @@
         <v>35</v>
       </c>
       <c r="D173" s="7" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="E173" s="7"/>
-      <c r="F173" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="G173" s="7" t="s">
-        <v>287</v>
-      </c>
+      <c r="F173" s="7"/>
+      <c r="G173" s="7"/>
       <c r="H173" s="7"/>
     </row>
     <row r="174" s="4" customFormat="1" spans="1:8">
@@ -6047,15 +5962,21 @@
         <v>173</v>
       </c>
       <c r="B174" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C174" s="6"/>
-      <c r="D174" s="6"/>
-      <c r="E174" s="6">
-        <v>5</v>
-      </c>
-      <c r="F174" s="6"/>
-      <c r="G174" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="C174" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D174" s="6" t="s">
+        <v>291</v>
+      </c>
+      <c r="E174" s="6"/>
+      <c r="F174" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="G174" s="6" t="s">
+        <v>176</v>
+      </c>
       <c r="H174" s="6"/>
     </row>
     <row r="175" s="4" customFormat="1" spans="1:8">
@@ -6063,23 +5984,19 @@
         <v>174</v>
       </c>
       <c r="B175" s="7" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C175" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D175" s="7" t="s">
-        <v>322</v>
-      </c>
-      <c r="E175" s="7" t="s">
-        <v>323</v>
-      </c>
-      <c r="F175" s="7" t="s">
-        <v>324</v>
-      </c>
-      <c r="G175" s="7" t="s">
-        <v>325</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="E175" s="7">
+        <v>200</v>
+      </c>
+      <c r="F175" s="7"/>
+      <c r="G175" s="7"/>
       <c r="H175" s="7"/>
     </row>
     <row r="176" s="4" customFormat="1" spans="1:8">
@@ -6090,14 +6007,18 @@
         <v>14</v>
       </c>
       <c r="C176" s="6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D176" s="6" t="s">
-        <v>326</v>
+        <v>293</v>
       </c>
       <c r="E176" s="6"/>
-      <c r="F176" s="6"/>
-      <c r="G176" s="6"/>
+      <c r="F176" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G176" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="H176" s="6"/>
     </row>
     <row r="177" s="4" customFormat="1" spans="1:8">
@@ -6110,7 +6031,7 @@
       <c r="C177" s="7"/>
       <c r="D177" s="7"/>
       <c r="E177" s="7">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F177" s="7"/>
       <c r="G177" s="7"/>
@@ -6121,16 +6042,16 @@
         <v>177</v>
       </c>
       <c r="B178" s="6" t="s">
-        <v>327</v>
+        <v>67</v>
       </c>
       <c r="C178" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D178" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="E178" s="6">
-        <v>10002</v>
+        <v>263</v>
+      </c>
+      <c r="E178" s="6" t="s">
+        <v>264</v>
       </c>
       <c r="F178" s="6"/>
       <c r="G178" s="6"/>
@@ -6141,17 +6062,23 @@
         <v>178</v>
       </c>
       <c r="B179" s="7" t="s">
-        <v>14</v>
+        <v>271</v>
       </c>
       <c r="C179" s="7" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D179" s="7" t="s">
-        <v>326</v>
-      </c>
-      <c r="E179" s="7"/>
-      <c r="F179" s="7"/>
-      <c r="G179" s="7"/>
+        <v>272</v>
+      </c>
+      <c r="E179" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="F179" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="G179" s="7" t="s">
+        <v>275</v>
+      </c>
       <c r="H179" s="7"/>
     </row>
     <row r="180" s="4" customFormat="1" spans="1:8">
@@ -6159,15 +6086,21 @@
         <v>179</v>
       </c>
       <c r="B180" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C180" s="6"/>
-      <c r="D180" s="6"/>
-      <c r="E180" s="6">
-        <v>1</v>
-      </c>
-      <c r="F180" s="6"/>
-      <c r="G180" s="6"/>
+        <v>14</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D180" s="6" t="s">
+        <v>293</v>
+      </c>
+      <c r="E180" s="6"/>
+      <c r="F180" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="G180" s="6" t="s">
+        <v>93</v>
+      </c>
       <c r="H180" s="6"/>
     </row>
     <row r="181" s="4" customFormat="1" spans="1:8">
@@ -6175,15 +6108,13 @@
         <v>180</v>
       </c>
       <c r="B181" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C181" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D181" s="7" t="s">
-        <v>329</v>
-      </c>
-      <c r="E181" s="7"/>
+        <v>11</v>
+      </c>
+      <c r="C181" s="7"/>
+      <c r="D181" s="7"/>
+      <c r="E181" s="7">
+        <v>2</v>
+      </c>
       <c r="F181" s="7"/>
       <c r="G181" s="7"/>
       <c r="H181" s="7"/>
@@ -6196,15 +6127,13 @@
         <v>14</v>
       </c>
       <c r="C182" s="6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D182" s="6" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="E182" s="6"/>
-      <c r="F182" s="6" t="s">
-        <v>289</v>
-      </c>
+      <c r="F182" s="6"/>
       <c r="G182" s="6"/>
       <c r="H182" s="6"/>
     </row>
@@ -6213,12 +6142,16 @@
         <v>182</v>
       </c>
       <c r="B183" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C183" s="7"/>
-      <c r="D183" s="7"/>
-      <c r="E183" s="7">
-        <v>3</v>
+        <v>67</v>
+      </c>
+      <c r="C183" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D183" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="E183" s="7" t="s">
+        <v>99</v>
       </c>
       <c r="F183" s="7"/>
       <c r="G183" s="7"/>
@@ -6235,7 +6168,7 @@
         <v>35</v>
       </c>
       <c r="D184" s="6" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="E184" s="6"/>
       <c r="F184" s="6"/>
@@ -6252,7 +6185,7 @@
       <c r="C185" s="7"/>
       <c r="D185" s="7"/>
       <c r="E185" s="7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F185" s="7"/>
       <c r="G185" s="7"/>
@@ -6263,22 +6196,16 @@
         <v>185</v>
       </c>
       <c r="B186" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C186" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D186" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="E186" s="6" t="s">
-        <v>292</v>
-      </c>
+        <v>278</v>
+      </c>
+      <c r="C186" s="6"/>
+      <c r="D186" s="6"/>
+      <c r="E186" s="6"/>
       <c r="F186" s="6" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="G186" s="6" t="s">
-        <v>105</v>
+        <v>298</v>
       </c>
       <c r="H186" s="6"/>
     </row>
@@ -6287,23 +6214,15 @@
         <v>186</v>
       </c>
       <c r="B187" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C187" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D187" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="E187" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="F187" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G187" s="7" t="s">
-        <v>34</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C187" s="7"/>
+      <c r="D187" s="7"/>
+      <c r="E187" s="7">
+        <v>10</v>
+      </c>
+      <c r="F187" s="7"/>
+      <c r="G187" s="7"/>
       <c r="H187" s="7"/>
     </row>
     <row r="188" s="4" customFormat="1" spans="1:8">
@@ -6311,20 +6230,20 @@
         <v>187</v>
       </c>
       <c r="B188" s="6" t="s">
-        <v>14</v>
+        <v>302</v>
       </c>
       <c r="C188" s="6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D188" s="6" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="E188" s="6"/>
       <c r="F188" s="6" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="G188" s="6" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="H188" s="6"/>
     </row>
@@ -6333,18 +6252,20 @@
         <v>188</v>
       </c>
       <c r="B189" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C189" s="7"/>
-      <c r="D189" s="7"/>
-      <c r="E189" s="7">
-        <v>4</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C189" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D189" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="E189" s="7"/>
       <c r="F189" s="7" t="s">
-        <v>12</v>
+        <v>286</v>
       </c>
       <c r="G189" s="7" t="s">
-        <v>13</v>
+        <v>287</v>
       </c>
       <c r="H189" s="7"/>
     </row>
@@ -6353,21 +6274,15 @@
         <v>189</v>
       </c>
       <c r="B190" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C190" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D190" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="E190" s="6"/>
-      <c r="F190" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="G190" s="6" t="s">
-        <v>301</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C190" s="6"/>
+      <c r="D190" s="6"/>
+      <c r="E190" s="6">
+        <v>5</v>
+      </c>
+      <c r="F190" s="6"/>
+      <c r="G190" s="6"/>
       <c r="H190" s="6"/>
     </row>
     <row r="191" s="4" customFormat="1" spans="1:8">
@@ -6375,20 +6290,22 @@
         <v>190</v>
       </c>
       <c r="B191" s="7" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="C191" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D191" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="E191" s="7"/>
+        <v>306</v>
+      </c>
+      <c r="E191" s="7" t="s">
+        <v>198</v>
+      </c>
       <c r="F191" s="7" t="s">
-        <v>303</v>
+        <v>314</v>
       </c>
       <c r="G191" s="7" t="s">
-        <v>304</v>
+        <v>309</v>
       </c>
       <c r="H191" s="7"/>
     </row>
@@ -6397,12 +6314,16 @@
         <v>191</v>
       </c>
       <c r="B192" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C192" s="6"/>
-      <c r="D192" s="6"/>
-      <c r="E192" s="6">
-        <v>1</v>
+        <v>67</v>
+      </c>
+      <c r="C192" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D192" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="E192" s="6" t="s">
+        <v>316</v>
       </c>
       <c r="F192" s="6"/>
       <c r="G192" s="6"/>
@@ -6413,15 +6334,17 @@
         <v>192</v>
       </c>
       <c r="B193" s="7" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="C193" s="7" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D193" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="E193" s="7"/>
+        <v>317</v>
+      </c>
+      <c r="E193" s="7" t="s">
+        <v>318</v>
+      </c>
       <c r="F193" s="7"/>
       <c r="G193" s="7"/>
       <c r="H193" s="7"/>
@@ -6431,21 +6354,19 @@
         <v>193</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C194" s="6" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D194" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="E194" s="6"/>
-      <c r="F194" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G194" s="6" t="s">
-        <v>176</v>
-      </c>
+        <v>319</v>
+      </c>
+      <c r="E194" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="F194" s="6"/>
+      <c r="G194" s="6"/>
       <c r="H194" s="6"/>
     </row>
     <row r="195" s="4" customFormat="1" spans="1:8">
@@ -6453,15 +6374,17 @@
         <v>194</v>
       </c>
       <c r="B195" s="7" t="s">
-        <v>14</v>
+        <v>320</v>
       </c>
       <c r="C195" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D195" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="E195" s="7"/>
+        <v>321</v>
+      </c>
+      <c r="E195" s="7">
+        <v>2</v>
+      </c>
       <c r="F195" s="7"/>
       <c r="G195" s="7"/>
       <c r="H195" s="7"/>
@@ -6471,21 +6394,19 @@
         <v>195</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>14</v>
+        <v>311</v>
       </c>
       <c r="C196" s="6" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D196" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="E196" s="6"/>
-      <c r="F196" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G196" s="6" t="s">
-        <v>176</v>
-      </c>
+        <v>312</v>
+      </c>
+      <c r="E196" s="6">
+        <v>10002</v>
+      </c>
+      <c r="F196" s="6"/>
+      <c r="G196" s="6"/>
       <c r="H196" s="6"/>
     </row>
     <row r="197" s="4" customFormat="1" spans="1:8">
@@ -6493,16 +6414,12 @@
         <v>196</v>
       </c>
       <c r="B197" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C197" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D197" s="7" t="s">
-        <v>309</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C197" s="7"/>
+      <c r="D197" s="7"/>
       <c r="E197" s="7">
-        <v>200</v>
+        <v>1</v>
       </c>
       <c r="F197" s="7"/>
       <c r="G197" s="7"/>
@@ -6519,15 +6436,11 @@
         <v>35</v>
       </c>
       <c r="D198" s="6" t="s">
-        <v>310</v>
+        <v>288</v>
       </c>
       <c r="E198" s="6"/>
-      <c r="F198" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G198" s="6" t="s">
-        <v>93</v>
-      </c>
+      <c r="F198" s="6"/>
+      <c r="G198" s="6"/>
       <c r="H198" s="6"/>
     </row>
     <row r="199" s="4" customFormat="1" spans="1:8">
@@ -6535,15 +6448,21 @@
         <v>198</v>
       </c>
       <c r="B199" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C199" s="7"/>
-      <c r="D199" s="7"/>
-      <c r="E199" s="7">
-        <v>3</v>
-      </c>
-      <c r="F199" s="7"/>
-      <c r="G199" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="C199" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D199" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="E199" s="7"/>
+      <c r="F199" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G199" s="7" t="s">
+        <v>176</v>
+      </c>
       <c r="H199" s="7"/>
     </row>
     <row r="200" s="4" customFormat="1" spans="1:8">
@@ -6551,17 +6470,15 @@
         <v>199</v>
       </c>
       <c r="B200" s="6" t="s">
-        <v>67</v>
+        <v>14</v>
       </c>
       <c r="C200" s="6" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="D200" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="E200" s="6" t="s">
-        <v>264</v>
-      </c>
+        <v>290</v>
+      </c>
+      <c r="E200" s="6"/>
       <c r="F200" s="6"/>
       <c r="G200" s="6"/>
       <c r="H200" s="6"/>
@@ -6571,22 +6488,20 @@
         <v>200</v>
       </c>
       <c r="B201" s="7" t="s">
-        <v>271</v>
+        <v>14</v>
       </c>
       <c r="C201" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D201" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="E201" s="7" t="s">
-        <v>273</v>
-      </c>
+        <v>291</v>
+      </c>
+      <c r="E201" s="7"/>
       <c r="F201" s="7" t="s">
-        <v>274</v>
+        <v>175</v>
       </c>
       <c r="G201" s="7" t="s">
-        <v>275</v>
+        <v>176</v>
       </c>
       <c r="H201" s="7"/>
     </row>
@@ -6595,21 +6510,19 @@
         <v>201</v>
       </c>
       <c r="B202" s="6" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C202" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D202" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="E202" s="6"/>
-      <c r="F202" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G202" s="6" t="s">
-        <v>93</v>
-      </c>
+        <v>292</v>
+      </c>
+      <c r="E202" s="6">
+        <v>200</v>
+      </c>
+      <c r="F202" s="6"/>
+      <c r="G202" s="6"/>
       <c r="H202" s="6"/>
     </row>
     <row r="203" s="4" customFormat="1" spans="1:8">
@@ -6617,15 +6530,21 @@
         <v>202</v>
       </c>
       <c r="B203" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C203" s="7"/>
-      <c r="D203" s="7"/>
-      <c r="E203" s="7">
-        <v>2</v>
-      </c>
-      <c r="F203" s="7"/>
-      <c r="G203" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="C203" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D203" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="E203" s="7"/>
+      <c r="F203" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G203" s="7" t="s">
+        <v>93</v>
+      </c>
       <c r="H203" s="7"/>
     </row>
     <row r="204" s="4" customFormat="1" spans="1:8">
@@ -6633,15 +6552,13 @@
         <v>203</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C204" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D204" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="E204" s="6"/>
+        <v>11</v>
+      </c>
+      <c r="C204" s="6"/>
+      <c r="D204" s="6"/>
+      <c r="E204" s="6">
+        <v>3</v>
+      </c>
       <c r="F204" s="6"/>
       <c r="G204" s="6"/>
       <c r="H204" s="6"/>
@@ -6654,13 +6571,13 @@
         <v>67</v>
       </c>
       <c r="C205" s="7" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="D205" s="7" t="s">
-        <v>312</v>
+        <v>263</v>
       </c>
       <c r="E205" s="7" t="s">
-        <v>99</v>
+        <v>264</v>
       </c>
       <c r="F205" s="7"/>
       <c r="G205" s="7"/>
@@ -6671,17 +6588,23 @@
         <v>205</v>
       </c>
       <c r="B206" s="6" t="s">
-        <v>14</v>
+        <v>271</v>
       </c>
       <c r="C206" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D206" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="E206" s="6"/>
-      <c r="F206" s="6"/>
-      <c r="G206" s="6"/>
+        <v>272</v>
+      </c>
+      <c r="E206" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="F206" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="G206" s="6" t="s">
+        <v>275</v>
+      </c>
       <c r="H206" s="6"/>
     </row>
     <row r="207" s="4" customFormat="1" spans="1:8">
@@ -6689,15 +6612,21 @@
         <v>206</v>
       </c>
       <c r="B207" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C207" s="7"/>
-      <c r="D207" s="7"/>
-      <c r="E207" s="7">
-        <v>10</v>
-      </c>
-      <c r="F207" s="7"/>
-      <c r="G207" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="C207" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D207" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="E207" s="7"/>
+      <c r="F207" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="G207" s="7" t="s">
+        <v>93</v>
+      </c>
       <c r="H207" s="7"/>
     </row>
     <row r="208" s="4" customFormat="1" spans="1:8">
@@ -6705,17 +6634,15 @@
         <v>207</v>
       </c>
       <c r="B208" s="6" t="s">
-        <v>278</v>
+        <v>11</v>
       </c>
       <c r="C208" s="6"/>
       <c r="D208" s="6"/>
-      <c r="E208" s="6"/>
-      <c r="F208" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="G208" s="6" t="s">
-        <v>314</v>
-      </c>
+      <c r="E208" s="6">
+        <v>2</v>
+      </c>
+      <c r="F208" s="6"/>
+      <c r="G208" s="6"/>
       <c r="H208" s="6"/>
     </row>
     <row r="209" s="4" customFormat="1" spans="1:8">
@@ -6723,13 +6650,15 @@
         <v>208</v>
       </c>
       <c r="B209" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C209" s="7"/>
-      <c r="D209" s="7"/>
-      <c r="E209" s="7">
-        <v>10</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="C209" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D209" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E209" s="7"/>
       <c r="F209" s="7"/>
       <c r="G209" s="7"/>
       <c r="H209" s="7"/>
@@ -6739,21 +6668,19 @@
         <v>209</v>
       </c>
       <c r="B210" s="6" t="s">
-        <v>233</v>
+        <v>67</v>
       </c>
       <c r="C210" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D210" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="E210" s="6"/>
-      <c r="F210" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="G210" s="6" t="s">
-        <v>317</v>
-      </c>
+        <v>295</v>
+      </c>
+      <c r="E210" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F210" s="6"/>
+      <c r="G210" s="6"/>
       <c r="H210" s="6"/>
     </row>
     <row r="211" s="4" customFormat="1" spans="1:8">
@@ -6761,21 +6688,17 @@
         <v>210</v>
       </c>
       <c r="B211" s="7" t="s">
-        <v>318</v>
+        <v>14</v>
       </c>
       <c r="C211" s="7" t="s">
         <v>35</v>
       </c>
       <c r="D211" s="7" t="s">
-        <v>319</v>
+        <v>294</v>
       </c>
       <c r="E211" s="7"/>
-      <c r="F211" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="G211" s="7" t="s">
-        <v>321</v>
-      </c>
+      <c r="F211" s="7"/>
+      <c r="G211" s="7"/>
       <c r="H211" s="7"/>
     </row>
     <row r="212" s="4" customFormat="1" spans="1:8">
@@ -6783,21 +6706,15 @@
         <v>211</v>
       </c>
       <c r="B212" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C212" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D212" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="E212" s="6"/>
-      <c r="F212" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="G212" s="6" t="s">
-        <v>287</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C212" s="6"/>
+      <c r="D212" s="6"/>
+      <c r="E212" s="6">
+        <v>10</v>
+      </c>
+      <c r="F212" s="6"/>
+      <c r="G212" s="6"/>
       <c r="H212" s="6"/>
     </row>
     <row r="213" s="4" customFormat="1" spans="1:8">
@@ -6805,15 +6722,17 @@
         <v>212</v>
       </c>
       <c r="B213" s="7" t="s">
-        <v>11</v>
+        <v>278</v>
       </c>
       <c r="C213" s="7"/>
       <c r="D213" s="7"/>
-      <c r="E213" s="7">
-        <v>5</v>
-      </c>
-      <c r="F213" s="7"/>
-      <c r="G213" s="7"/>
+      <c r="E213" s="7"/>
+      <c r="F213" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="G213" s="7" t="s">
+        <v>298</v>
+      </c>
       <c r="H213" s="7"/>
     </row>
     <row r="214" s="4" customFormat="1" spans="1:8">
@@ -6821,762 +6740,26 @@
         <v>213</v>
       </c>
       <c r="B214" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C214" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D214" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="E214" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="F214" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="G214" s="6" t="s">
-        <v>325</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="C214" s="6"/>
+      <c r="D214" s="6"/>
+      <c r="E214" s="6">
+        <v>10</v>
+      </c>
+      <c r="F214" s="6"/>
+      <c r="G214" s="6"/>
       <c r="H214" s="6"/>
-    </row>
-    <row r="215" s="4" customFormat="1" spans="1:8">
-      <c r="A215" s="7">
-        <v>214</v>
-      </c>
-      <c r="B215" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C215" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D215" s="7" t="s">
-        <v>331</v>
-      </c>
-      <c r="E215" s="7" t="s">
-        <v>332</v>
-      </c>
-      <c r="F215" s="7"/>
-      <c r="G215" s="7"/>
-      <c r="H215" s="7"/>
-    </row>
-    <row r="216" s="4" customFormat="1" spans="1:8">
-      <c r="A216" s="6">
-        <v>215</v>
-      </c>
-      <c r="B216" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C216" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D216" s="6" t="s">
-        <v>333</v>
-      </c>
-      <c r="E216" s="6" t="s">
-        <v>334</v>
-      </c>
-      <c r="F216" s="6"/>
-      <c r="G216" s="6"/>
-      <c r="H216" s="6"/>
-    </row>
-    <row r="217" s="4" customFormat="1" spans="1:8">
-      <c r="A217" s="7">
-        <v>216</v>
-      </c>
-      <c r="B217" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C217" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D217" s="7" t="s">
-        <v>335</v>
-      </c>
-      <c r="E217" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="F217" s="7"/>
-      <c r="G217" s="7"/>
-      <c r="H217" s="7"/>
-    </row>
-    <row r="218" s="4" customFormat="1" spans="1:8">
-      <c r="A218" s="6">
-        <v>217</v>
-      </c>
-      <c r="B218" s="6" t="s">
-        <v>336</v>
-      </c>
-      <c r="C218" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D218" s="6" t="s">
-        <v>337</v>
-      </c>
-      <c r="E218" s="6">
-        <v>2</v>
-      </c>
-      <c r="F218" s="6"/>
-      <c r="G218" s="6"/>
-      <c r="H218" s="6"/>
-    </row>
-    <row r="219" s="4" customFormat="1" spans="1:8">
-      <c r="A219" s="7">
-        <v>218</v>
-      </c>
-      <c r="B219" s="7" t="s">
-        <v>327</v>
-      </c>
-      <c r="C219" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D219" s="7" t="s">
-        <v>328</v>
-      </c>
-      <c r="E219" s="7">
-        <v>10002</v>
-      </c>
-      <c r="F219" s="7"/>
-      <c r="G219" s="7"/>
-      <c r="H219" s="7"/>
-    </row>
-    <row r="220" s="4" customFormat="1" spans="1:8">
-      <c r="A220" s="6">
-        <v>219</v>
-      </c>
-      <c r="B220" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C220" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D220" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="E220" s="6"/>
-      <c r="F220" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="G220" s="6"/>
-      <c r="H220" s="6"/>
-    </row>
-    <row r="221" s="4" customFormat="1" spans="1:8">
-      <c r="A221" s="7">
-        <v>220</v>
-      </c>
-      <c r="B221" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C221" s="7"/>
-      <c r="D221" s="7"/>
-      <c r="E221" s="7">
-        <v>3</v>
-      </c>
-      <c r="F221" s="7"/>
-      <c r="G221" s="7"/>
-      <c r="H221" s="7"/>
-    </row>
-    <row r="222" s="4" customFormat="1" spans="1:8">
-      <c r="A222" s="6">
-        <v>221</v>
-      </c>
-      <c r="B222" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C222" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D222" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="E222" s="6"/>
-      <c r="F222" s="6"/>
-      <c r="G222" s="6"/>
-      <c r="H222" s="6"/>
-    </row>
-    <row r="223" s="4" customFormat="1" spans="1:8">
-      <c r="A223" s="7">
-        <v>222</v>
-      </c>
-      <c r="B223" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C223" s="7"/>
-      <c r="D223" s="7"/>
-      <c r="E223" s="7">
-        <v>1</v>
-      </c>
-      <c r="F223" s="7"/>
-      <c r="G223" s="7"/>
-      <c r="H223" s="7"/>
-    </row>
-    <row r="224" s="4" customFormat="1" spans="1:8">
-      <c r="A224" s="6">
-        <v>223</v>
-      </c>
-      <c r="B224" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C224" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D224" s="6" t="s">
-        <v>291</v>
-      </c>
-      <c r="E224" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="F224" s="6" t="s">
-        <v>293</v>
-      </c>
-      <c r="G224" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="H224" s="6"/>
-    </row>
-    <row r="225" s="4" customFormat="1" spans="1:8">
-      <c r="A225" s="7">
-        <v>224</v>
-      </c>
-      <c r="B225" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C225" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D225" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="E225" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="F225" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="G225" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="H225" s="7"/>
-    </row>
-    <row r="226" s="4" customFormat="1" spans="1:8">
-      <c r="A226" s="6">
-        <v>225</v>
-      </c>
-      <c r="B226" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C226" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D226" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="E226" s="6"/>
-      <c r="F226" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="G226" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="H226" s="6"/>
-    </row>
-    <row r="227" s="4" customFormat="1" spans="1:8">
-      <c r="A227" s="7">
-        <v>226</v>
-      </c>
-      <c r="B227" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C227" s="7"/>
-      <c r="D227" s="7"/>
-      <c r="E227" s="7">
-        <v>4</v>
-      </c>
-      <c r="F227" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G227" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="H227" s="7"/>
-    </row>
-    <row r="228" s="4" customFormat="1" spans="1:8">
-      <c r="A228" s="6">
-        <v>227</v>
-      </c>
-      <c r="B228" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C228" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D228" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="E228" s="6"/>
-      <c r="F228" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="G228" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="H228" s="6"/>
-    </row>
-    <row r="229" s="4" customFormat="1" spans="1:8">
-      <c r="A229" s="7">
-        <v>228</v>
-      </c>
-      <c r="B229" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C229" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D229" s="7" t="s">
-        <v>302</v>
-      </c>
-      <c r="E229" s="7"/>
-      <c r="F229" s="7" t="s">
-        <v>303</v>
-      </c>
-      <c r="G229" s="7" t="s">
-        <v>304</v>
-      </c>
-      <c r="H229" s="7"/>
-    </row>
-    <row r="230" s="4" customFormat="1" spans="1:8">
-      <c r="A230" s="6">
-        <v>229</v>
-      </c>
-      <c r="B230" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C230" s="6"/>
-      <c r="D230" s="6"/>
-      <c r="E230" s="6">
-        <v>1</v>
-      </c>
-      <c r="F230" s="6"/>
-      <c r="G230" s="6"/>
-      <c r="H230" s="6"/>
-    </row>
-    <row r="231" s="4" customFormat="1" spans="1:8">
-      <c r="A231" s="7">
-        <v>230</v>
-      </c>
-      <c r="B231" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C231" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D231" s="7" t="s">
-        <v>305</v>
-      </c>
-      <c r="E231" s="7"/>
-      <c r="F231" s="7"/>
-      <c r="G231" s="7"/>
-      <c r="H231" s="7"/>
-    </row>
-    <row r="232" s="4" customFormat="1" spans="1:8">
-      <c r="A232" s="6">
-        <v>231</v>
-      </c>
-      <c r="B232" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C232" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D232" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="E232" s="6"/>
-      <c r="F232" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G232" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H232" s="6"/>
-    </row>
-    <row r="233" s="4" customFormat="1" spans="1:8">
-      <c r="A233" s="7">
-        <v>232</v>
-      </c>
-      <c r="B233" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C233" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D233" s="7" t="s">
-        <v>307</v>
-      </c>
-      <c r="E233" s="7"/>
-      <c r="F233" s="7"/>
-      <c r="G233" s="7"/>
-      <c r="H233" s="7"/>
-    </row>
-    <row r="234" s="4" customFormat="1" spans="1:8">
-      <c r="A234" s="6">
-        <v>233</v>
-      </c>
-      <c r="B234" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C234" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D234" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="E234" s="6"/>
-      <c r="F234" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="G234" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="H234" s="6"/>
-    </row>
-    <row r="235" s="4" customFormat="1" spans="1:8">
-      <c r="A235" s="7">
-        <v>234</v>
-      </c>
-      <c r="B235" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C235" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D235" s="7" t="s">
-        <v>309</v>
-      </c>
-      <c r="E235" s="7">
-        <v>200</v>
-      </c>
-      <c r="F235" s="7"/>
-      <c r="G235" s="7"/>
-      <c r="H235" s="7"/>
-    </row>
-    <row r="236" s="4" customFormat="1" spans="1:8">
-      <c r="A236" s="6">
-        <v>235</v>
-      </c>
-      <c r="B236" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C236" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D236" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="E236" s="6"/>
-      <c r="F236" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G236" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H236" s="6"/>
-    </row>
-    <row r="237" s="4" customFormat="1" spans="1:8">
-      <c r="A237" s="7">
-        <v>236</v>
-      </c>
-      <c r="B237" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C237" s="7"/>
-      <c r="D237" s="7"/>
-      <c r="E237" s="7">
-        <v>3</v>
-      </c>
-      <c r="F237" s="7"/>
-      <c r="G237" s="7"/>
-      <c r="H237" s="7"/>
-    </row>
-    <row r="238" s="4" customFormat="1" spans="1:8">
-      <c r="A238" s="6">
-        <v>237</v>
-      </c>
-      <c r="B238" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="C238" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D238" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="E238" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="F238" s="6"/>
-      <c r="G238" s="6"/>
-      <c r="H238" s="6"/>
-    </row>
-    <row r="239" s="4" customFormat="1" spans="1:8">
-      <c r="A239" s="7">
-        <v>238</v>
-      </c>
-      <c r="B239" s="7" t="s">
-        <v>271</v>
-      </c>
-      <c r="C239" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D239" s="7" t="s">
-        <v>272</v>
-      </c>
-      <c r="E239" s="7" t="s">
-        <v>273</v>
-      </c>
-      <c r="F239" s="7" t="s">
-        <v>274</v>
-      </c>
-      <c r="G239" s="7" t="s">
-        <v>275</v>
-      </c>
-      <c r="H239" s="7"/>
-    </row>
-    <row r="240" s="4" customFormat="1" spans="1:8">
-      <c r="A240" s="6">
-        <v>239</v>
-      </c>
-      <c r="B240" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C240" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D240" s="6" t="s">
-        <v>310</v>
-      </c>
-      <c r="E240" s="6"/>
-      <c r="F240" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="G240" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="H240" s="6"/>
-    </row>
-    <row r="241" s="4" customFormat="1" spans="1:8">
-      <c r="A241" s="7">
-        <v>240</v>
-      </c>
-      <c r="B241" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C241" s="7"/>
-      <c r="D241" s="7"/>
-      <c r="E241" s="7">
-        <v>2</v>
-      </c>
-      <c r="F241" s="7"/>
-      <c r="G241" s="7"/>
-      <c r="H241" s="7"/>
-    </row>
-    <row r="242" s="4" customFormat="1" spans="1:8">
-      <c r="A242" s="6">
-        <v>241</v>
-      </c>
-      <c r="B242" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C242" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D242" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="E242" s="6"/>
-      <c r="F242" s="6"/>
-      <c r="G242" s="6"/>
-      <c r="H242" s="6"/>
-    </row>
-    <row r="243" s="4" customFormat="1" spans="1:8">
-      <c r="A243" s="7">
-        <v>242</v>
-      </c>
-      <c r="B243" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="C243" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D243" s="7" t="s">
-        <v>312</v>
-      </c>
-      <c r="E243" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="F243" s="7"/>
-      <c r="G243" s="7"/>
-      <c r="H243" s="7"/>
-    </row>
-    <row r="244" s="4" customFormat="1" spans="1:8">
-      <c r="A244" s="6">
-        <v>243</v>
-      </c>
-      <c r="B244" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C244" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D244" s="6" t="s">
-        <v>311</v>
-      </c>
-      <c r="E244" s="6"/>
-      <c r="F244" s="6"/>
-      <c r="G244" s="6"/>
-      <c r="H244" s="6"/>
-    </row>
-    <row r="245" s="4" customFormat="1" spans="1:8">
-      <c r="A245" s="7">
-        <v>244</v>
-      </c>
-      <c r="B245" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C245" s="7"/>
-      <c r="D245" s="7"/>
-      <c r="E245" s="7">
-        <v>10</v>
-      </c>
-      <c r="F245" s="7"/>
-      <c r="G245" s="7"/>
-      <c r="H245" s="7"/>
-    </row>
-    <row r="246" s="4" customFormat="1" spans="1:8">
-      <c r="A246" s="6">
-        <v>245</v>
-      </c>
-      <c r="B246" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="C246" s="6"/>
-      <c r="D246" s="6"/>
-      <c r="E246" s="6"/>
-      <c r="F246" s="6" t="s">
-        <v>313</v>
-      </c>
-      <c r="G246" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="H246" s="6"/>
-    </row>
-    <row r="247" s="4" customFormat="1" spans="1:8">
-      <c r="A247" s="7">
-        <v>246</v>
-      </c>
-      <c r="B247" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C247" s="7"/>
-      <c r="D247" s="7"/>
-      <c r="E247" s="7">
-        <v>10</v>
-      </c>
-      <c r="F247" s="7"/>
-      <c r="G247" s="7"/>
-      <c r="H247" s="7"/>
-    </row>
-    <row r="248" s="4" customFormat="1" spans="1:8">
-      <c r="A248" s="6">
-        <v>247</v>
-      </c>
-      <c r="B248" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="C248" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D248" s="6" t="s">
-        <v>315</v>
-      </c>
-      <c r="E248" s="6"/>
-      <c r="F248" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="G248" s="6" t="s">
-        <v>317</v>
-      </c>
-      <c r="H248" s="6"/>
-    </row>
-    <row r="249" s="4" customFormat="1" spans="1:8">
-      <c r="A249" s="7">
-        <v>248</v>
-      </c>
-      <c r="B249" s="7" t="s">
-        <v>318</v>
-      </c>
-      <c r="C249" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D249" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="E249" s="7"/>
-      <c r="F249" s="7" t="s">
-        <v>320</v>
-      </c>
-      <c r="G249" s="7" t="s">
-        <v>321</v>
-      </c>
-      <c r="H249" s="7"/>
-    </row>
-    <row r="250" spans="1:8">
-      <c r="A250" s="7">
-        <v>250</v>
-      </c>
-      <c r="B250" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C250" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D250" s="7" t="s">
-        <v>338</v>
-      </c>
-      <c r="E250" s="7"/>
-      <c r="F250" s="7" t="s">
-        <v>339</v>
-      </c>
-      <c r="G250" s="7" t="s">
-        <v>340</v>
-      </c>
-      <c r="H250" s="7"/>
-    </row>
-    <row r="251" spans="1:8">
-      <c r="A251" s="8">
-        <v>251</v>
-      </c>
-      <c r="B251" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C251" s="6"/>
-      <c r="D251" s="6"/>
-      <c r="E251" s="6">
-        <v>4</v>
-      </c>
-      <c r="F251" s="6"/>
-      <c r="G251" s="6"/>
-      <c r="H251" s="6"/>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B142 B173 B174 B179 B212 B213 B216 B217 B218 B219 B1:B141 B143:B144 B145:B146 B154:B163 B164:B172 B175:B176 B177:B178 B180:B181 B182:B183 B184:B185 B193:B202 B203:B211 B214:B215 B220:B221 B222:B223 B231:B240 B241:B249 B250:B1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B142 B162 B163 B168 B188 B189 B190 B193 B194 B195 B196 B1:B141 B143:B152 B153:B161 B164:B165 B166:B167 B169:B170 B171:B180 B181:B187 B191:B192 B198:B207 B208:B214 B215:B1048576">
       <formula1>DataList!$C$2:$C$109</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C173 C179 C180 C212 C218 C219 C1:C141 C142:C144 C145:C146 C154:C163 C164:C172 C174:C176 C177:C178 C182:C183 C184:C185 C193:C202 C203:C211 C213:C215 C216:C217 C220:C221 C222:C223 C231:C240 C241:C249 C250:C1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C142 C162 C168 C169 C188 C189 C195 C196 C1:C141 C143:C152 C153:C161 C163:C165 C166:C167 C171:C180 C181:C187 C190:C192 C193:C194 C198:C207 C208:C214 C215:C1048576">
       <formula1>DataList!$A$2:$A$14</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B147:B153 B186:B192 B224:B230">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B197">
       <formula1>[1]DataList!#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -7607,7 +6790,7 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>341</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -7615,20 +6798,20 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>342</v>
+        <v>323</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
-        <v>343</v>
+        <v>324</v>
       </c>
       <c r="C3" t="s">
-        <v>344</v>
+        <v>325</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" t="s">
-        <v>345</v>
+        <v>326</v>
       </c>
       <c r="C4" t="s">
         <v>11</v>
@@ -7639,20 +6822,20 @@
         <v>35</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>346</v>
+        <v>327</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" t="s">
-        <v>347</v>
+        <v>328</v>
       </c>
       <c r="C6" t="s">
-        <v>348</v>
+        <v>329</v>
       </c>
     </row>
     <row r="7" spans="1:3">
       <c r="A7" t="s">
-        <v>349</v>
+        <v>330</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -7660,47 +6843,47 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
       <c r="C8" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
     </row>
     <row r="10" spans="1:3">
       <c r="A10" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="C10" t="s">
-        <v>356</v>
+        <v>337</v>
       </c>
     </row>
     <row r="11" spans="1:3">
       <c r="A11" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="C11" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
     </row>
     <row r="12" spans="3:3">
       <c r="C12" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
     </row>
     <row r="13" spans="3:3">
       <c r="C13" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
     </row>
     <row r="14" spans="3:3">
@@ -7710,12 +6893,12 @@
     </row>
     <row r="15" spans="3:3">
       <c r="C15" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="3:3">
       <c r="C16" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
     </row>
     <row r="17" spans="3:3">
@@ -7725,17 +6908,17 @@
     </row>
     <row r="18" spans="3:3">
       <c r="C18" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="3:3">
       <c r="C19" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
     </row>
     <row r="20" spans="3:3">
       <c r="C20" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
     </row>
     <row r="21" spans="3:3">
@@ -7745,35 +6928,35 @@
     </row>
     <row r="22" spans="3:3">
       <c r="C22" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
     </row>
     <row r="23" spans="3:4">
       <c r="C23" s="2" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
     </row>
     <row r="24" spans="3:3">
       <c r="C24" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25" spans="3:3">
       <c r="C25" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
     </row>
     <row r="26" spans="3:3">
       <c r="C26" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
     </row>
     <row r="27" spans="3:3">
       <c r="C27" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
     </row>
     <row r="28" spans="3:3">
@@ -7783,62 +6966,62 @@
     </row>
     <row r="29" spans="3:3">
       <c r="C29" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
     </row>
     <row r="30" spans="3:3">
       <c r="C30" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
     </row>
     <row r="31" spans="3:3">
       <c r="C31" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
     </row>
     <row r="32" spans="3:3">
       <c r="C32" t="s">
-        <v>373</v>
+        <v>354</v>
       </c>
     </row>
     <row r="33" spans="3:3">
       <c r="C33" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
     </row>
     <row r="34" spans="3:3">
       <c r="C34" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
     </row>
     <row r="35" spans="3:3">
       <c r="C35" t="s">
-        <v>376</v>
+        <v>357</v>
       </c>
     </row>
     <row r="36" spans="3:3">
       <c r="C36" t="s">
-        <v>377</v>
+        <v>358</v>
       </c>
     </row>
     <row r="37" spans="3:3">
       <c r="C37" t="s">
-        <v>378</v>
+        <v>359</v>
       </c>
     </row>
     <row r="38" spans="3:3">
       <c r="C38" t="s">
-        <v>379</v>
+        <v>360</v>
       </c>
     </row>
     <row r="39" spans="3:3">
       <c r="C39" t="s">
-        <v>380</v>
+        <v>361</v>
       </c>
     </row>
     <row r="40" spans="3:3">
       <c r="C40" t="s">
-        <v>381</v>
+        <v>362</v>
       </c>
     </row>
     <row r="41" spans="3:3">
@@ -7848,87 +7031,87 @@
     </row>
     <row r="42" spans="3:3">
       <c r="C42" t="s">
-        <v>382</v>
+        <v>363</v>
       </c>
     </row>
     <row r="43" spans="3:3">
       <c r="C43" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
     </row>
     <row r="44" spans="3:3">
       <c r="C44" t="s">
-        <v>384</v>
+        <v>365</v>
       </c>
     </row>
     <row r="45" spans="3:3">
       <c r="C45" t="s">
-        <v>385</v>
+        <v>366</v>
       </c>
     </row>
     <row r="46" spans="3:3">
       <c r="C46" t="s">
-        <v>386</v>
+        <v>367</v>
       </c>
     </row>
     <row r="47" spans="3:3">
       <c r="C47" t="s">
-        <v>387</v>
+        <v>368</v>
       </c>
     </row>
     <row r="48" spans="3:3">
       <c r="C48" t="s">
-        <v>388</v>
+        <v>369</v>
       </c>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" t="s">
-        <v>389</v>
+        <v>370</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
     </row>
     <row r="51" spans="3:3">
       <c r="C51" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
     </row>
     <row r="52" spans="3:3">
       <c r="C52" t="s">
-        <v>392</v>
+        <v>373</v>
       </c>
     </row>
     <row r="53" spans="3:3">
       <c r="C53" t="s">
-        <v>393</v>
+        <v>374</v>
       </c>
     </row>
     <row r="54" spans="3:3">
       <c r="C54" t="s">
-        <v>394</v>
+        <v>375</v>
       </c>
     </row>
     <row r="55" spans="3:3">
       <c r="C55" t="s">
-        <v>395</v>
+        <v>376</v>
       </c>
     </row>
     <row r="56" spans="3:3">
       <c r="C56" t="s">
-        <v>396</v>
+        <v>377</v>
       </c>
     </row>
     <row r="57" spans="3:3">
       <c r="C57" t="s">
-        <v>397</v>
+        <v>378</v>
       </c>
     </row>
     <row r="58" spans="3:3">
       <c r="C58" t="s">
-        <v>398</v>
+        <v>379</v>
       </c>
     </row>
     <row r="59" spans="3:3">
@@ -7938,199 +7121,199 @@
     </row>
     <row r="60" spans="3:3">
       <c r="C60" t="s">
-        <v>399</v>
+        <v>380</v>
       </c>
     </row>
     <row r="61" spans="3:3">
       <c r="C61" t="s">
-        <v>400</v>
+        <v>381</v>
       </c>
     </row>
     <row r="62" spans="3:3">
       <c r="C62" t="s">
-        <v>401</v>
+        <v>382</v>
       </c>
     </row>
     <row r="63" spans="3:3">
       <c r="C63" t="s">
-        <v>402</v>
+        <v>383</v>
       </c>
     </row>
     <row r="64" spans="3:3">
       <c r="C64" t="s">
-        <v>403</v>
+        <v>384</v>
       </c>
     </row>
     <row r="65" spans="3:3">
       <c r="C65" t="s">
-        <v>404</v>
+        <v>385</v>
       </c>
     </row>
     <row r="66" spans="3:3">
       <c r="C66" t="s">
-        <v>405</v>
+        <v>386</v>
       </c>
     </row>
     <row r="67" spans="3:3">
       <c r="C67" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
     </row>
     <row r="68" spans="3:3">
       <c r="C68" t="s">
-        <v>406</v>
+        <v>387</v>
       </c>
     </row>
     <row r="69" spans="3:3">
       <c r="C69" t="s">
-        <v>407</v>
+        <v>388</v>
       </c>
     </row>
     <row r="70" spans="3:3">
       <c r="C70" t="s">
-        <v>408</v>
+        <v>389</v>
       </c>
     </row>
     <row r="71" spans="3:4">
       <c r="C71" s="2" t="s">
-        <v>409</v>
+        <v>390</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
     </row>
     <row r="72" spans="3:3">
       <c r="C72" t="s">
-        <v>410</v>
+        <v>391</v>
       </c>
     </row>
     <row r="73" spans="3:4">
       <c r="C73" s="2" t="s">
-        <v>411</v>
+        <v>392</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
     </row>
     <row r="74" spans="3:3">
       <c r="C74" t="s">
-        <v>412</v>
+        <v>393</v>
       </c>
     </row>
     <row r="75" spans="3:3">
       <c r="C75" t="s">
-        <v>413</v>
+        <v>394</v>
       </c>
     </row>
     <row r="76" spans="3:3">
       <c r="C76" t="s">
-        <v>414</v>
+        <v>395</v>
       </c>
     </row>
     <row r="77" spans="3:3">
       <c r="C77" t="s">
-        <v>415</v>
+        <v>396</v>
       </c>
     </row>
     <row r="78" spans="3:4">
       <c r="C78" s="2" t="s">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
     </row>
     <row r="79" spans="3:4">
       <c r="C79" s="2" t="s">
-        <v>417</v>
+        <v>398</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
     </row>
     <row r="80" spans="3:3">
       <c r="C80" t="s">
-        <v>418</v>
+        <v>399</v>
       </c>
     </row>
     <row r="81" spans="3:3">
       <c r="C81" t="s">
-        <v>419</v>
+        <v>400</v>
       </c>
     </row>
     <row r="82" spans="3:3">
       <c r="C82" t="s">
-        <v>420</v>
+        <v>401</v>
       </c>
     </row>
     <row r="83" spans="3:3">
       <c r="C83" t="s">
-        <v>421</v>
+        <v>402</v>
       </c>
     </row>
     <row r="84" spans="3:3">
       <c r="C84" t="s">
-        <v>422</v>
+        <v>403</v>
       </c>
     </row>
     <row r="85" spans="3:3">
       <c r="C85" t="s">
-        <v>423</v>
+        <v>404</v>
       </c>
     </row>
     <row r="86" spans="3:3">
       <c r="C86" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
     </row>
     <row r="87" spans="3:3">
       <c r="C87" t="s">
-        <v>425</v>
+        <v>406</v>
       </c>
     </row>
     <row r="88" spans="3:3">
       <c r="C88" t="s">
-        <v>426</v>
+        <v>407</v>
       </c>
     </row>
     <row r="89" spans="3:3">
       <c r="C89" t="s">
-        <v>427</v>
+        <v>408</v>
       </c>
     </row>
     <row r="90" spans="3:3">
       <c r="C90" t="s">
-        <v>428</v>
+        <v>409</v>
       </c>
     </row>
     <row r="91" spans="3:3">
       <c r="C91" t="s">
-        <v>429</v>
+        <v>410</v>
       </c>
     </row>
     <row r="92" spans="3:3">
       <c r="C92" t="s">
-        <v>430</v>
+        <v>411</v>
       </c>
     </row>
     <row r="93" spans="3:3">
       <c r="C93" t="s">
-        <v>431</v>
+        <v>412</v>
       </c>
     </row>
     <row r="94" spans="3:3">
       <c r="C94" t="s">
-        <v>432</v>
+        <v>413</v>
       </c>
     </row>
     <row r="95" spans="3:3">
       <c r="C95" t="s">
-        <v>433</v>
+        <v>414</v>
       </c>
     </row>
     <row r="96" spans="3:3">
       <c r="C96" s="3" t="s">
-        <v>434</v>
+        <v>415</v>
       </c>
     </row>
     <row r="97" spans="3:3">
@@ -8145,17 +7328,17 @@
     </row>
     <row r="99" spans="3:3">
       <c r="C99" t="s">
-        <v>435</v>
+        <v>416</v>
       </c>
     </row>
     <row r="100" spans="3:3">
       <c r="C100" t="s">
-        <v>436</v>
+        <v>417</v>
       </c>
     </row>
     <row r="101" spans="3:3">
       <c r="C101" t="s">
-        <v>437</v>
+        <v>418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>